<commit_message>
maj projet 3 + java
</commit_message>
<xml_diff>
--- a/Projet_3(Back-end)/Budget/Budget.xlsx
+++ b/Projet_3(Back-end)/Budget/Budget.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\D_documents\OpenClassroom\OC\Projet_3(Back-end)\Budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="17256" windowHeight="6120"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="17256" windowHeight="6120"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Print_Area" localSheetId="0">Feuil1!$A$1:$K$41</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Tâches</t>
   </si>
@@ -105,6 +108,9 @@
   </si>
   <si>
     <t>Bénéfice</t>
+  </si>
+  <si>
+    <t>Facturé</t>
   </si>
 </sst>
 </file>
@@ -674,56 +680,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -766,12 +730,82 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1080,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I26"/>
+  <dimension ref="B1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,9 +1125,7 @@
     <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.21875" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1105,11 +1137,11 @@
       <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="45"/>
+      <c r="F2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -1127,34 +1159,34 @@
         <v>5</v>
       </c>
       <c r="C3" s="11">
-        <f>C19/220</f>
-        <v>238.58181818181819</v>
-      </c>
-      <c r="D3" s="31">
-        <f>D19/220</f>
-        <v>245.45454545454547</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="15" t="s">
+        <f>(C19/220)*2</f>
+        <v>196.36363636363637</v>
+      </c>
+      <c r="D3" s="20">
+        <f>(D19/220)*2</f>
+        <v>327.27272727272725</v>
+      </c>
+      <c r="E3" s="46"/>
+      <c r="F3" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="53">
-        <v>1.2</v>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="39">
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="16"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="15"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
@@ -1164,22 +1196,22 @@
       <c r="D5" s="2">
         <v>0.5</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="47">
+      <c r="E5" s="46"/>
+      <c r="F5" s="33">
         <f>$C$3*C5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="37">
         <f>$D$3*D5</f>
-        <v>122.72727272727273</v>
-      </c>
-      <c r="H5" s="48">
+        <v>163.63636363636363</v>
+      </c>
+      <c r="H5" s="34">
         <f>SUM(F5:G5)</f>
-        <v>122.72727272727273</v>
-      </c>
-      <c r="I5" s="17">
+        <v>163.63636363636363</v>
+      </c>
+      <c r="I5" s="16">
         <f>H5*$I$3</f>
-        <v>147.27272727272728</v>
+        <v>188.18181818181816</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
@@ -1190,22 +1222,22 @@
       <c r="D6" s="2">
         <v>1</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="47">
+      <c r="E6" s="46"/>
+      <c r="F6" s="33">
         <f t="shared" ref="F6:F15" si="0">$C$3*C6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="37">
         <f t="shared" ref="G6:G15" si="1">$D$3*D6</f>
-        <v>245.45454545454547</v>
-      </c>
-      <c r="H6" s="48">
+        <v>327.27272727272725</v>
+      </c>
+      <c r="H6" s="34">
         <f t="shared" ref="H6:H15" si="2">SUM(F6:G6)</f>
-        <v>245.45454545454547</v>
-      </c>
-      <c r="I6" s="17">
+        <v>327.27272727272725</v>
+      </c>
+      <c r="I6" s="16">
         <f t="shared" ref="I6:I15" si="3">H6*$I$3</f>
-        <v>294.54545454545456</v>
+        <v>376.36363636363632</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
@@ -1216,35 +1248,35 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="47">
+      <c r="E7" s="46"/>
+      <c r="F7" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="37">
         <f t="shared" si="1"/>
-        <v>245.45454545454547</v>
-      </c>
-      <c r="H7" s="48">
+        <v>327.27272727272725</v>
+      </c>
+      <c r="H7" s="34">
         <f t="shared" si="2"/>
-        <v>245.45454545454547</v>
-      </c>
-      <c r="I7" s="17">
+        <v>327.27272727272725</v>
+      </c>
+      <c r="I7" s="16">
         <f t="shared" si="3"/>
-        <v>294.54545454545456</v>
+        <v>376.36363636363632</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="18"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
@@ -1256,22 +1288,22 @@
       <c r="D9" s="2">
         <v>0.5</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="47">
+      <c r="E9" s="46"/>
+      <c r="F9" s="33">
         <f t="shared" si="0"/>
-        <v>119.2909090909091</v>
-      </c>
-      <c r="G9" s="51">
+        <v>98.181818181818187</v>
+      </c>
+      <c r="G9" s="37">
         <f t="shared" si="1"/>
-        <v>122.72727272727273</v>
-      </c>
-      <c r="H9" s="48">
+        <v>163.63636363636363</v>
+      </c>
+      <c r="H9" s="34">
         <f t="shared" si="2"/>
-        <v>242.01818181818183</v>
-      </c>
-      <c r="I9" s="17">
+        <v>261.81818181818181</v>
+      </c>
+      <c r="I9" s="16">
         <f t="shared" si="3"/>
-        <v>290.4218181818182</v>
+        <v>301.09090909090907</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -1282,35 +1314,35 @@
       <c r="D10" s="2">
         <v>0.2</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="47">
+      <c r="E10" s="46"/>
+      <c r="F10" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="37">
         <f t="shared" si="1"/>
-        <v>49.090909090909093</v>
-      </c>
-      <c r="H10" s="48">
+        <v>65.454545454545453</v>
+      </c>
+      <c r="H10" s="34">
         <f t="shared" si="2"/>
-        <v>49.090909090909093</v>
-      </c>
-      <c r="I10" s="17">
+        <v>65.454545454545453</v>
+      </c>
+      <c r="I10" s="16">
         <f t="shared" si="3"/>
-        <v>58.909090909090907</v>
+        <v>75.272727272727266</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="18"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
@@ -1320,22 +1352,22 @@
         <v>2</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="47">
+      <c r="E12" s="46"/>
+      <c r="F12" s="33">
         <f t="shared" si="0"/>
-        <v>477.16363636363639</v>
-      </c>
-      <c r="G12" s="51">
+        <v>392.72727272727275</v>
+      </c>
+      <c r="G12" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="34">
         <f t="shared" si="2"/>
-        <v>477.16363636363639</v>
-      </c>
-      <c r="I12" s="17">
+        <v>392.72727272727275</v>
+      </c>
+      <c r="I12" s="16">
         <f t="shared" si="3"/>
-        <v>572.59636363636366</v>
+        <v>451.63636363636363</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
@@ -1348,22 +1380,22 @@
       <c r="D13" s="2">
         <v>0.5</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="47">
+      <c r="E13" s="46"/>
+      <c r="F13" s="33">
         <f t="shared" si="0"/>
-        <v>119.2909090909091</v>
-      </c>
-      <c r="G13" s="51">
+        <v>98.181818181818187</v>
+      </c>
+      <c r="G13" s="37">
         <f t="shared" si="1"/>
-        <v>122.72727272727273</v>
-      </c>
-      <c r="H13" s="48">
+        <v>163.63636363636363</v>
+      </c>
+      <c r="H13" s="34">
         <f t="shared" si="2"/>
-        <v>242.01818181818183</v>
-      </c>
-      <c r="I13" s="17">
+        <v>261.81818181818181</v>
+      </c>
+      <c r="I13" s="16">
         <f t="shared" si="3"/>
-        <v>290.4218181818182</v>
+        <v>301.09090909090907</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -1374,22 +1406,22 @@
         <v>1</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="47">
+      <c r="E14" s="46"/>
+      <c r="F14" s="33">
         <f t="shared" si="0"/>
-        <v>238.58181818181819</v>
-      </c>
-      <c r="G14" s="51">
+        <v>196.36363636363637</v>
+      </c>
+      <c r="G14" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H14" s="48">
+      <c r="H14" s="34">
         <f t="shared" si="2"/>
-        <v>238.58181818181819</v>
-      </c>
-      <c r="I14" s="17">
+        <v>196.36363636363637</v>
+      </c>
+      <c r="I14" s="16">
         <f t="shared" si="3"/>
-        <v>286.29818181818183</v>
+        <v>225.81818181818181</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1399,135 +1431,145 @@
       <c r="C15" s="5">
         <v>0.5</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="49">
+      <c r="D15" s="21"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="35">
         <f t="shared" si="0"/>
-        <v>119.2909090909091</v>
-      </c>
-      <c r="G15" s="52">
+        <v>98.181818181818187</v>
+      </c>
+      <c r="G15" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="50">
+      <c r="H15" s="36">
         <f t="shared" si="2"/>
-        <v>119.2909090909091</v>
-      </c>
-      <c r="I15" s="19">
+        <v>98.181818181818187</v>
+      </c>
+      <c r="I15" s="18">
         <f t="shared" si="3"/>
-        <v>143.14909090909092</v>
+        <v>112.90909090909091</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E16" s="35"/>
+      <c r="E16" s="46"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="45">
-        <v>2916</v>
-      </c>
-      <c r="D17" s="46">
-        <v>3000</v>
-      </c>
-      <c r="E17" s="35"/>
+      <c r="C17" s="31">
+        <v>1200</v>
+      </c>
+      <c r="D17" s="32">
+        <v>2000</v>
+      </c>
+      <c r="E17" s="46"/>
     </row>
     <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="33">
         <f>C17*1.5</f>
-        <v>4374</v>
-      </c>
-      <c r="D18" s="48">
+        <v>1800</v>
+      </c>
+      <c r="D18" s="34">
         <f>D17*1.5</f>
-        <v>4500</v>
-      </c>
-      <c r="E18" s="35"/>
+        <v>3000</v>
+      </c>
+      <c r="E18" s="46"/>
     </row>
     <row r="19" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="49">
+      <c r="C19" s="35">
         <f>C18*12</f>
-        <v>52488</v>
-      </c>
-      <c r="D19" s="50">
+        <v>21600</v>
+      </c>
+      <c r="D19" s="36">
         <f>D18*12</f>
-        <v>54000</v>
-      </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="54" t="s">
+        <v>36000</v>
+      </c>
+      <c r="E19" s="46"/>
+      <c r="F19" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="55" t="s">
+      <c r="G19" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="56" t="s">
+      <c r="H19" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="38" t="s">
+      <c r="I19" s="24" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="44">
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="30">
         <f>SUM(F5:F15)</f>
-        <v>1073.6181818181819</v>
-      </c>
-      <c r="G20" s="43">
+        <v>883.63636363636374</v>
+      </c>
+      <c r="G20" s="29">
         <f>SUM(G5:G15)</f>
-        <v>908.18181818181824</v>
-      </c>
-      <c r="H20" s="42">
+        <v>1210.909090909091</v>
+      </c>
+      <c r="H20" s="28">
         <f>SUM(F20:G20)</f>
-        <v>1981.8000000000002</v>
-      </c>
-      <c r="I20" s="40">
+        <v>2094.545454545455</v>
+      </c>
+      <c r="I20" s="26">
         <f>SUM(I5:I15)</f>
-        <v>2378.1600000000003</v>
+        <v>2408.7272727272725</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I21" s="39" t="s">
+      <c r="I21" s="25" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="I22" s="40">
+      <c r="I22" s="26">
         <f>I20*0.2</f>
-        <v>475.63200000000006</v>
+        <v>481.74545454545455</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I23" s="39" t="s">
+      <c r="I23" s="25" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="I24" s="40">
+      <c r="I24" s="26">
         <f>I20+I22</f>
-        <v>2853.7920000000004</v>
+        <v>2890.4727272727268</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="I25" s="37" t="s">
+      <c r="I25" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="I26" s="41">
+      <c r="I26" s="27">
         <f>I20-H20</f>
-        <v>396.36000000000013</v>
+        <v>314.18181818181756</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="I27" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="I28" s="26">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
@@ -1543,6 +1585,9 @@
     <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="11" max="40" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>